<commit_message>
hovSerialAdapter: Add 3D models from SnapEDA.
Add 3D models from SnapEDA to the footprints of the RJ-45 jack, and for the 8.2uH inductivity
</commit_message>
<xml_diff>
--- a/hovSerialAdapter/hovSerialAdapter_BOM.xlsx
+++ b/hovSerialAdapter/hovSerialAdapter_BOM.xlsx
@@ -254,15 +254,6 @@
     <t>8.2uH</t>
   </si>
   <si>
-    <t>FIXED IND 8.2UH 1.3A 128 MOHM</t>
-  </si>
-  <si>
-    <t>490-16860-1-ND</t>
-  </si>
-  <si>
-    <t>LQH43PN8R2M26L</t>
-  </si>
-  <si>
     <t xml:space="preserve">    L5</t>
   </si>
   <si>
@@ -402,6 +393,15 @@
   </si>
   <si>
     <t>Qty</t>
+  </si>
+  <si>
+    <t>FIXED IND 8.2UH 1.3A 153.6 MOHM</t>
+  </si>
+  <si>
+    <t>490-16115-1-ND</t>
+  </si>
+  <si>
+    <t>LQH43PH8R2M26L</t>
   </si>
 </sst>
 </file>
@@ -723,7 +723,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,25 +738,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
         <v>119</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>120</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>121</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>122</v>
-      </c>
-      <c r="E1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1085,13 +1085,13 @@
         <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F17" t="s">
         <v>63</v>
@@ -1102,19 +1102,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" t="s">
         <v>79</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E18" t="s">
         <v>80</v>
-      </c>
-      <c r="C18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" t="s">
-        <v>83</v>
       </c>
       <c r="F18" t="s">
         <v>63</v>
@@ -1125,10 +1125,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1136,22 +1136,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B20" s="1">
         <v>43952</v>
       </c>
       <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" t="s">
         <v>87</v>
-      </c>
-      <c r="D20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" t="s">
-        <v>89</v>
-      </c>
-      <c r="F20" t="s">
-        <v>90</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1159,22 +1159,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B21">
         <v>100</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1182,22 +1182,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
         <v>95</v>
       </c>
-      <c r="B22" t="s">
+      <c r="E22" t="s">
         <v>96</v>
       </c>
-      <c r="C22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" t="s">
-        <v>99</v>
-      </c>
       <c r="F22" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1205,10 +1205,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1216,10 +1216,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1227,22 +1227,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" t="s">
         <v>104</v>
       </c>
-      <c r="B25" t="s">
+      <c r="E25" t="s">
         <v>105</v>
       </c>
-      <c r="C25" t="s">
+      <c r="F25" t="s">
         <v>106</v>
-      </c>
-      <c r="D25" t="s">
-        <v>107</v>
-      </c>
-      <c r="E25" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" t="s">
-        <v>109</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1250,22 +1250,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" t="s">
         <v>110</v>
       </c>
-      <c r="B26" t="s">
-        <v>111</v>
-      </c>
-      <c r="C26" t="s">
-        <v>112</v>
-      </c>
-      <c r="D26" t="s">
-        <v>113</v>
-      </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1273,22 +1273,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" t="s">
         <v>114</v>
       </c>
-      <c r="B27" t="s">
+      <c r="E27" t="s">
         <v>115</v>
       </c>
-      <c r="C27" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" t="s">
-        <v>118</v>
-      </c>
       <c r="F27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G27">
         <v>1</v>

</xml_diff>

<commit_message>
Serial adapter: Update BOM
</commit_message>
<xml_diff>
--- a/hovSerialAdapter/hovSerialAdapter_BOM.xlsx
+++ b/hovSerialAdapter/hovSerialAdapter_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="127">
   <si>
     <t xml:space="preserve">    C1</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>LQH43PH8R2M26L</t>
+  </si>
+  <si>
+    <t>1.5</t>
   </si>
 </sst>
 </file>
@@ -437,9 +440,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,581 +728,606 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G10">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G12">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="1">
-        <v>43952</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>100</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G23">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G24">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="83" orientation="landscape" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>